<commit_message>
Fixing more wiki typos
</commit_message>
<xml_diff>
--- a/opinions/parsed_wiki_data/1999.xlsx
+++ b/opinions/parsed_wiki_data/1999.xlsx
@@ -487,47 +487,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -537,47 +537,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -587,47 +587,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -637,47 +637,47 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -687,47 +687,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -737,47 +737,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -787,47 +787,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -837,47 +837,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -887,47 +887,47 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -937,12 +937,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -987,47 +987,47 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority  </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1047,12 +1047,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1087,47 +1087,47 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1137,47 +1137,47 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrencedissent </t>
+          <t>concurrencedissent</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrencedissent  </t>
+          <t>joinconcurrencedissent</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrencedissent </t>
+          <t>joinconcurrencedissent</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrencedissent  </t>
+          <t>joinconcurrencedissent</t>
         </is>
       </c>
     </row>
@@ -1187,47 +1187,47 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1237,22 +1237,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1262,17 +1262,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1297,12 +1297,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1312,22 +1312,22 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1337,47 +1337,47 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1387,47 +1387,47 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoindissent  </t>
+          <t>partjoindissent</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
     </row>
@@ -1437,47 +1437,47 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1497,27 +1497,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
     </row>
@@ -1537,27 +1537,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1567,17 +1567,17 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority  </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1597,22 +1597,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrencedissent  </t>
+          <t>concurrencedissent</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1647,27 +1647,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1687,47 +1687,47 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1737,47 +1737,47 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1787,47 +1787,47 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1847,17 +1847,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1887,37 +1887,37 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
     </row>
@@ -1937,47 +1937,47 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -1987,42 +1987,42 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2057,27 +2057,27 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -2087,47 +2087,47 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2137,47 +2137,47 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -2187,47 +2187,47 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2237,47 +2237,47 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
     </row>
@@ -2287,47 +2287,47 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2337,47 +2337,47 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2387,47 +2387,47 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -2437,47 +2437,47 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2492,17 +2492,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2512,22 +2512,22 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2567,12 +2567,12 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2587,47 +2587,47 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">didnotparticipate </t>
+          <t>didnotparticipate</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2637,47 +2637,47 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
     </row>
@@ -2687,42 +2687,42 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2787,47 +2787,47 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2837,47 +2837,47 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
     </row>
@@ -2887,47 +2887,47 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority  </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2972,7 +2972,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -2987,47 +2987,47 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3037,47 +3037,47 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3087,17 +3087,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -3107,7 +3107,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3147,17 +3147,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3187,47 +3187,47 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3237,22 +3237,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3262,22 +3262,22 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3287,12 +3287,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3302,17 +3302,17 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3322,12 +3322,12 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -3337,47 +3337,47 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
     </row>
@@ -3387,42 +3387,42 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3457,12 +3457,12 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3472,12 +3472,12 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3507,12 +3507,12 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3522,12 +3522,12 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3537,47 +3537,47 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -3587,47 +3587,47 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3637,47 +3637,47 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3737,47 +3737,47 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality  </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">plurality </t>
+          <t>plurality</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence  </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality  </t>
+          <t>joinplurality</t>
         </is>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3802,12 +3802,12 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
     </row>
@@ -3837,47 +3837,47 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">partjoinmajority </t>
+          <t>partjoinmajority</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -3887,37 +3887,37 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -3937,47 +3937,47 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality  </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t xml:space="preserve">plurality </t>
+          <t>plurality</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality  </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
     </row>
@@ -3987,47 +3987,47 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4037,47 +4037,47 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4087,47 +4087,47 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
     </row>
@@ -4137,47 +4137,47 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4187,27 +4187,27 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
     </row>
@@ -4237,47 +4237,47 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4287,47 +4287,47 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrencedissent  </t>
+          <t>concurrencedissent</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrencedissent </t>
+          <t>joinconcurrencedissent</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrencedissent  </t>
+          <t>joinconcurrencedissent</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4337,47 +4337,47 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4392,12 +4392,12 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -4407,12 +4407,12 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4422,7 +4422,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -4437,22 +4437,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4462,22 +4462,22 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
     </row>
@@ -4487,47 +4487,47 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
     </row>
@@ -4537,27 +4537,27 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority  </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -4567,7 +4567,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -4587,12 +4587,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinmajority  </t>
+          <t>joinmajority</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">majority </t>
+          <t>majority</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -4602,12 +4602,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent  </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4637,47 +4637,47 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality  </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t xml:space="preserve">concurrence </t>
+          <t>concurrence</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinplurality </t>
+          <t>joinplurality</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t xml:space="preserve">dissent  </t>
+          <t>dissent</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t xml:space="preserve">plurality  </t>
+          <t>plurality</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joindissent </t>
+          <t>joindissent</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t xml:space="preserve">joinconcurrence  </t>
+          <t>joinconcurrence</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally updated opinions since 1999
</commit_message>
<xml_diff>
--- a/opinions/parsed_wiki_data/1999.xlsx
+++ b/opinions/parsed_wiki_data/1999.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -497,37 +497,37 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,37 +547,37 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -597,37 +597,37 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -647,37 +647,37 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -697,37 +697,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -737,47 +737,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -797,37 +797,37 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -837,47 +837,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -887,42 +887,42 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -947,37 +947,37 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -987,37 +987,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1037,12 +1037,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1052,32 +1052,32 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -1087,17 +1087,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1107,27 +1107,27 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1142,42 +1142,42 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>concurrence dissent concurrencedissent</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>joinconcurrencedissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>joinconcurrencedissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>joinconcurrencedissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -1192,42 +1192,42 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1257,27 +1257,27 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
     </row>
@@ -1287,17 +1287,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1307,17 +1307,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1337,47 +1337,47 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1397,37 +1397,37 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>partjoindissent</t>
+          <t>dissent partjoindissent joindissent</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -1437,27 +1437,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1467,17 +1467,17 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1487,34 +1487,34 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>dissent joindissent</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>majority joinmajority</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>majority joinmajority</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>majority joinmajority</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>dissent</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>joinmajority</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>joinmajority</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>joinmajority</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>dissent</t>
-        </is>
-      </c>
       <c r="H22" t="inlineStr">
         <is>
           <t>majority</t>
@@ -1522,12 +1522,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -1537,17 +1537,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1557,17 +1557,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1587,17 +1587,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1607,27 +1607,27 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>concurrence dissent concurrencedissent</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>partjoinmajority majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence joindissent</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -1637,22 +1637,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1672,12 +1672,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
     </row>
@@ -1687,32 +1687,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1722,12 +1722,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1737,37 +1737,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1787,42 +1787,42 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -1837,12 +1837,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1852,32 +1852,32 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1897,12 +1897,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1912,17 +1912,17 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent partjoindissent joindissent</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -1937,27 +1937,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1967,17 +1967,17 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -1987,47 +1987,47 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
     </row>
@@ -2037,42 +2037,42 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>dissent joindissent</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>majority joinmajority</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>dissent partjoindissent joindissent</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>dissent joindissent</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>majority joinmajority</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
           <t>dissent</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>joinmajority</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>dissent</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>joindissent</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>joinmajority</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>dissent</t>
-        </is>
-      </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2087,22 +2087,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2112,22 +2112,22 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2157,17 +2157,17 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -2187,22 +2187,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2212,22 +2212,22 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2237,12 +2237,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2252,27 +2252,27 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2287,27 +2287,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2317,17 +2317,17 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2337,17 +2337,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2357,27 +2357,27 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2387,22 +2387,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2417,17 +2417,17 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -2437,17 +2437,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2467,17 +2467,17 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2487,37 +2487,37 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>majority</t>
+          <t>majority plurality</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2557,27 +2557,27 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
     </row>
@@ -2587,12 +2587,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2602,32 +2602,32 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2642,37 +2642,37 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2687,12 +2687,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2702,22 +2702,22 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
     </row>
@@ -2737,47 +2737,47 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>majority</t>
+          <t>majority plurality</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
     </row>
@@ -2787,22 +2787,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2812,22 +2812,22 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2837,17 +2837,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2857,22 +2857,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2887,37 +2887,37 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -2937,22 +2937,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2962,22 +2962,22 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2997,22 +2997,22 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3022,12 +3022,12 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3047,27 +3047,27 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3097,22 +3097,22 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>partjoinmajority majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3122,12 +3122,12 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -3142,42 +3142,42 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent partjoindissent joindissent</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent partjoindissent joindissent</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -3187,22 +3187,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3212,7 +3212,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3222,12 +3222,12 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3237,17 +3237,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3257,27 +3257,27 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
+          <t>partjoinmajority majority concurrence joinmajority</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>majority</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
           <t>concurrence</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>majority</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>concurrence</t>
-        </is>
-      </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3287,42 +3287,42 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -3342,22 +3342,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3367,17 +3367,17 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3407,17 +3407,17 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -3437,22 +3437,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3462,17 +3462,17 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -3487,37 +3487,37 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3547,32 +3547,32 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -3587,17 +3587,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3607,27 +3607,27 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3637,27 +3637,27 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3667,17 +3667,17 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3697,37 +3697,37 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3772,12 +3772,12 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
     </row>
@@ -3787,42 +3787,42 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>majority</t>
+          <t>majority plurality</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinplurality joinmajority plurality</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -3837,42 +3837,42 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority joinmajority</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -3887,12 +3887,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3902,32 +3902,32 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3952,7 +3952,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3962,22 +3962,22 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -3987,27 +3987,27 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -4017,17 +4017,17 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4037,32 +4037,32 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -4072,12 +4072,12 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4087,32 +4087,32 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4127,7 +4127,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -4147,37 +4147,37 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4187,12 +4187,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -4202,27 +4202,27 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinmajority</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>partjoinmajority</t>
+          <t>partjoinmajority majority concurrence dissent concurrencedissent joinconcurrencedissent joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -4237,17 +4237,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -4267,17 +4267,17 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4287,37 +4287,37 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>concurrencedissent</t>
+          <t>concurrence dissent concurrencedissent</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>joinconcurrencedissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>joinconcurrencedissent</t>
+          <t>concurrence dissent concurrencedissent joinconcurrencedissent joinconcurrence</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4342,12 +4342,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -4357,27 +4357,27 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -4402,32 +4402,32 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence partjoinconcurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4447,7 +4447,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -4457,27 +4457,27 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -4497,32 +4497,32 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -4547,37 +4547,37 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>dissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
     </row>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority joinmajority</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4612,22 +4612,22 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>concurrence</t>
+          <t>majority concurrence joinmajority</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>joinmajority</t>
+          <t>majority concurrence joinmajority joinconcurrence</t>
         </is>
       </c>
     </row>
@@ -4637,12 +4637,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -4652,12 +4652,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>joinplurality</t>
+          <t>joinplurality plurality</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4672,12 +4672,12 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>joindissent</t>
+          <t>dissent joindissent</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>joinconcurrence</t>
+          <t>concurrence joinconcurrence</t>
         </is>
       </c>
     </row>

</xml_diff>